<commit_message>
Modified the Chapter 1's Application Architecture, but haven't finished it yet
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Capstone 2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{26996BFE-AD7C-472F-88EC-A27EE71C05D0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{23219F8B-FB47-4898-8EA2-5D109DC06BBF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{83B6082E-9E44-41D9-BB0A-A25EEDCBCFB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>LIST OF SOURCES FOR THE CAPSTONE PROJECT DOCUMENTATION</t>
   </si>
@@ -49,13 +49,22 @@
   </si>
   <si>
     <t>Web Link not yet retrieved</t>
+  </si>
+  <si>
+    <t>General Web Architecture</t>
+  </si>
+  <si>
+    <t>1 - Project Overview</t>
+  </si>
+  <si>
+    <t>1 - Application Architecture</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +80,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -80,7 +96,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -108,26 +124,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -160,58 +156,43 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -530,95 +511,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B92398D7-C530-400B-B3F6-7F69DDE151A5}">
   <dimension ref="C4:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="40.140625" customWidth="1"/>
+    <col min="4" max="5" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C5" s="8"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5" t="s">
+      <c r="E6" s="9"/>
+      <c r="F6" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G6" s="6"/>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
       <c r="L6" s="6"/>
-      <c r="M6" s="5" t="s">
+      <c r="M6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
       <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="10">
-        <v>1</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11">
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="7">
         <v>43291</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
       <c r="M7" s="10" t="s">
         <v>7</v>
       </c>
@@ -628,216 +610,255 @@
       <c r="Q7" s="10"/>
     </row>
     <row r="8" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C8" s="9"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="7">
+        <v>43291</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="10" t="s">
+        <v>7</v>
+      </c>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
       <c r="P8" s="10"/>
       <c r="Q8" s="10"/>
     </row>
     <row r="9" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C9" s="9"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
     </row>
     <row r="10" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C10" s="9"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="10"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
     </row>
     <row r="11" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C11" s="9"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
     </row>
     <row r="12" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C12" s="9"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
     </row>
     <row r="13" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C13" s="9"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
     </row>
     <row r="14" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
     </row>
     <row r="15" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C15" s="9"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
     </row>
     <row r="16" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
     </row>
     <row r="17" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
     </row>
     <row r="18" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C18" s="9"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
     </row>
     <row r="19" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C19" s="9"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="M14:Q14"/>
-    <mergeCell ref="M15:Q15"/>
-    <mergeCell ref="M16:Q16"/>
-    <mergeCell ref="M17:Q17"/>
-    <mergeCell ref="M18:Q18"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="C4:Q5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="H8:L8"/>
+    <mergeCell ref="H9:L9"/>
+    <mergeCell ref="H10:L10"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="H12:L12"/>
     <mergeCell ref="M19:Q19"/>
     <mergeCell ref="H19:L19"/>
     <mergeCell ref="M6:Q6"/>
@@ -854,42 +875,11 @@
     <mergeCell ref="H16:L16"/>
     <mergeCell ref="H17:L17"/>
     <mergeCell ref="H18:L18"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="H8:L8"/>
-    <mergeCell ref="H9:L9"/>
-    <mergeCell ref="H10:L10"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="C4:Q5"/>
+    <mergeCell ref="M14:Q14"/>
+    <mergeCell ref="M15:Q15"/>
+    <mergeCell ref="M16:Q16"/>
+    <mergeCell ref="M17:Q17"/>
+    <mergeCell ref="M18:Q18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added the first two links for the sources
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Capstone 2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{23219F8B-FB47-4898-8EA2-5D109DC06BBF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DFA9B4B5-602B-4D82-8CA3-7CFDD3D9C564}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{83B6082E-9E44-41D9-BB0A-A25EEDCBCFB4}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>LIST OF SOURCES FOR THE CAPSTONE PROJECT DOCUMENTATION</t>
   </si>
@@ -58,13 +58,19 @@
   </si>
   <si>
     <t>1 - Application Architecture</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Web_application</t>
+  </si>
+  <si>
+    <t>http://www.woodger.ca/archweb.htm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +89,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -157,10 +171,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -172,31 +187,35 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -512,7 +531,7 @@
   <dimension ref="C4:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H9" sqref="H9:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,67 +541,67 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="4" t="s">
+      <c r="E6" s="5"/>
+      <c r="F6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="4" t="s">
+      <c r="G6" s="7"/>
+      <c r="H6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="4" t="s">
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="6"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="7"/>
     </row>
     <row r="7" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
@@ -592,22 +611,24 @@
         <v>9</v>
       </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="7">
+      <c r="F7" s="10">
         <v>43291</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="H7" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="10" t="s">
+      <c r="M7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
     </row>
     <row r="8" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
@@ -617,22 +638,24 @@
         <v>10</v>
       </c>
       <c r="E8" s="3"/>
-      <c r="F8" s="7">
+      <c r="F8" s="10">
         <v>43291</v>
       </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="H8" s="12" t="s">
+        <v>12</v>
+      </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="10" t="s">
+      <c r="M8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
     </row>
     <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
@@ -823,16 +846,37 @@
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="C4:Q5"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="M14:Q14"/>
+    <mergeCell ref="M15:Q15"/>
+    <mergeCell ref="M16:Q16"/>
+    <mergeCell ref="M17:Q17"/>
+    <mergeCell ref="M18:Q18"/>
+    <mergeCell ref="M19:Q19"/>
+    <mergeCell ref="H19:L19"/>
+    <mergeCell ref="M6:Q6"/>
+    <mergeCell ref="M7:Q7"/>
+    <mergeCell ref="M8:Q8"/>
+    <mergeCell ref="M9:Q9"/>
+    <mergeCell ref="M10:Q10"/>
+    <mergeCell ref="M11:Q11"/>
+    <mergeCell ref="M12:Q12"/>
+    <mergeCell ref="M13:Q13"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="H14:L14"/>
+    <mergeCell ref="H15:L15"/>
+    <mergeCell ref="H16:L16"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="H8:L8"/>
+    <mergeCell ref="H9:L9"/>
+    <mergeCell ref="H10:L10"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="H12:L12"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F8:G8"/>
@@ -849,39 +893,22 @@
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="H8:L8"/>
-    <mergeCell ref="H9:L9"/>
-    <mergeCell ref="H10:L10"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="M19:Q19"/>
-    <mergeCell ref="H19:L19"/>
-    <mergeCell ref="M6:Q6"/>
-    <mergeCell ref="M7:Q7"/>
-    <mergeCell ref="M8:Q8"/>
-    <mergeCell ref="M9:Q9"/>
-    <mergeCell ref="M10:Q10"/>
-    <mergeCell ref="M11:Q11"/>
-    <mergeCell ref="M12:Q12"/>
-    <mergeCell ref="M13:Q13"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="H14:L14"/>
-    <mergeCell ref="H15:L15"/>
-    <mergeCell ref="H16:L16"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="H18:L18"/>
-    <mergeCell ref="M14:Q14"/>
-    <mergeCell ref="M15:Q15"/>
-    <mergeCell ref="M16:Q16"/>
-    <mergeCell ref="M17:Q17"/>
-    <mergeCell ref="M18:Q18"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="C4:Q5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H7" r:id="rId1" xr:uid="{5F529AA9-04C6-4CFB-992F-811598F7BCCB}"/>
+    <hyperlink ref="H8" r:id="rId2" xr:uid="{0DA5ECA3-C672-4B56-A954-AC77135F9636}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made a new folder for Capstone docs and edited the Sources list
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Capstone 2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DFA9B4B5-602B-4D82-8CA3-7CFDD3D9C564}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{9BF821DF-24C3-4792-9891-372A00391FD0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{83B6082E-9E44-41D9-BB0A-A25EEDCBCFB4}"/>
   </bookViews>
@@ -54,16 +54,16 @@
     <t>General Web Architecture</t>
   </si>
   <si>
-    <t>1 - Project Overview</t>
-  </si>
-  <si>
-    <t>1 - Application Architecture</t>
-  </si>
-  <si>
     <t>https://en.wikipedia.org/wiki/Web_application</t>
   </si>
   <si>
     <t>http://www.woodger.ca/archweb.htm</t>
+  </si>
+  <si>
+    <t>Project Proposal - Application Architecture</t>
+  </si>
+  <si>
+    <t>Project Proposal - Project Overview</t>
   </si>
 </sst>
 </file>
@@ -187,30 +187,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -531,131 +531,131 @@
   <dimension ref="C4:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9:L9"/>
+      <selection activeCell="D8" sqref="D8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="40.140625" customWidth="1"/>
-    <col min="4" max="5" width="16.7109375" customWidth="1"/>
+    <col min="4" max="5" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="6" t="s">
+      <c r="G6" s="6"/>
+      <c r="H6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="6" t="s">
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="7"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="9">
+        <v>43291</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="10">
-        <v>43291</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="12" t="s">
-        <v>11</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="11" t="s">
+      <c r="M7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
     </row>
     <row r="8" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="9">
+        <v>43291</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="10">
-        <v>43291</v>
-      </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="12" t="s">
-        <v>12</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="11" t="s">
+      <c r="M8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
     </row>
     <row r="9" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
@@ -846,11 +846,42 @@
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="M14:Q14"/>
-    <mergeCell ref="M15:Q15"/>
-    <mergeCell ref="M16:Q16"/>
-    <mergeCell ref="M17:Q17"/>
-    <mergeCell ref="M18:Q18"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:L6"/>
+    <mergeCell ref="C4:Q5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="H8:L8"/>
+    <mergeCell ref="H9:L9"/>
+    <mergeCell ref="H10:L10"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="H12:L12"/>
     <mergeCell ref="M19:Q19"/>
     <mergeCell ref="H19:L19"/>
     <mergeCell ref="M6:Q6"/>
@@ -867,42 +898,11 @@
     <mergeCell ref="H16:L16"/>
     <mergeCell ref="H17:L17"/>
     <mergeCell ref="H18:L18"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H7:L7"/>
-    <mergeCell ref="H8:L8"/>
-    <mergeCell ref="H9:L9"/>
-    <mergeCell ref="H10:L10"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="H12:L12"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:L6"/>
-    <mergeCell ref="C4:Q5"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="M14:Q14"/>
+    <mergeCell ref="M15:Q15"/>
+    <mergeCell ref="M16:Q16"/>
+    <mergeCell ref="M17:Q17"/>
+    <mergeCell ref="M18:Q18"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H7" r:id="rId1" xr:uid="{5F529AA9-04C6-4CFB-992F-811598F7BCCB}"/>

</xml_diff>